<commit_message>
new mediators added. 60 sm words
</commit_message>
<xml_diff>
--- a/cue_target_pairs.xlsx
+++ b/cue_target_pairs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\pretest_fmri\guess\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\pretest_fmri\Guess_fMRI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AAC1CEE-726C-4B38-87CF-D3ABADBFD963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA058B4-6C71-498F-8ED0-B1B8E0B165C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="160">
   <si>
     <t>cue</t>
   </si>
@@ -381,12 +381,6 @@
     <t>Gold</t>
   </si>
   <si>
-    <t>Kamin</t>
-  </si>
-  <si>
-    <t>Ziegel</t>
-  </si>
-  <si>
     <t>Kante</t>
   </si>
   <si>
@@ -423,12 +417,6 @@
     <t>Straße</t>
   </si>
   <si>
-    <t>Rose</t>
-  </si>
-  <si>
-    <t>Dorne</t>
-  </si>
-  <si>
     <t>Schauspielerin</t>
   </si>
   <si>
@@ -499,6 +487,24 @@
   </si>
   <si>
     <t>Rolle</t>
+  </si>
+  <si>
+    <t>Surfen</t>
+  </si>
+  <si>
+    <t>Strand</t>
+  </si>
+  <si>
+    <t>Kastanien</t>
+  </si>
+  <si>
+    <t>Rösten</t>
+  </si>
+  <si>
+    <t>Nudeln</t>
+  </si>
+  <si>
+    <t>Pizza</t>
   </si>
 </sst>
 </file>
@@ -877,10 +883,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B79"/>
+  <dimension ref="A1:B80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1359,174 +1365,182 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A60" s="2" t="s">
-        <v>118</v>
+        <v>156</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>119</v>
+        <v>157</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A61" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A62" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A63" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A64" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A65" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A66" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A67" s="2" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>133</v>
+        <v>155</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A68" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A69" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A70" s="2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A71" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A72" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A73" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A74" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A75" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A76" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A77" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A78" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A79" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>157</v>
+        <v>153</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A80" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A79">
+  <conditionalFormatting sqref="A2:A80">
     <cfRule type="duplicateValues" dxfId="3" priority="2"/>
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B79">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  <conditionalFormatting sqref="A2:B80">
+    <cfRule type="duplicateValues" dxfId="1" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:B79">
-    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
+  <conditionalFormatting sqref="B2:B80">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
improved stim set - Lauras comments
</commit_message>
<xml_diff>
--- a/cue_target_pairs.xlsx
+++ b/cue_target_pairs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\pretest_fmri\Guess_fMRI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5545DB65-5EA8-41C8-9C19-F8EF08F98F42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927C19B5-481B-4D3C-B42F-0EB365BC255B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -90,9 +90,6 @@
     <t>Geburtstag</t>
   </si>
   <si>
-    <t>Kerze</t>
-  </si>
-  <si>
     <t>Geschwister</t>
   </si>
   <si>
@@ -135,12 +132,6 @@
     <t>Brise</t>
   </si>
   <si>
-    <t>Decke</t>
-  </si>
-  <si>
-    <t>Kissen</t>
-  </si>
-  <si>
     <t>Frieden</t>
   </si>
   <si>
@@ -159,12 +150,6 @@
     <t>Publikum</t>
   </si>
   <si>
-    <t>Pumpe</t>
-  </si>
-  <si>
-    <t>Reifen</t>
-  </si>
-  <si>
     <t>Raum</t>
   </si>
   <si>
@@ -255,9 +240,6 @@
     <t>Klinge</t>
   </si>
   <si>
-    <t>Station</t>
-  </si>
-  <si>
     <t>Erbe</t>
   </si>
   <si>
@@ -327,9 +309,6 @@
     <t>Schmerz</t>
   </si>
   <si>
-    <t>Gesellschaft</t>
-  </si>
-  <si>
     <t>Büro</t>
   </si>
   <si>
@@ -372,12 +351,6 @@
     <t>Asche</t>
   </si>
   <si>
-    <t>Kiefer</t>
-  </si>
-  <si>
-    <t>Kabine</t>
-  </si>
-  <si>
     <t>Rebe</t>
   </si>
   <si>
@@ -390,21 +363,12 @@
     <t>Sonntag</t>
   </si>
   <si>
-    <t>Milch</t>
-  </si>
-  <si>
-    <t>Butter</t>
-  </si>
-  <si>
     <t>Popcorn</t>
   </si>
   <si>
     <t>Wohnung</t>
   </si>
   <si>
-    <t>Handy</t>
-  </si>
-  <si>
     <t>Nummer</t>
   </si>
   <si>
@@ -511,6 +475,42 @@
   </si>
   <si>
     <t>Duft</t>
+  </si>
+  <si>
+    <t>Center</t>
+  </si>
+  <si>
+    <t>Kerzen</t>
+  </si>
+  <si>
+    <t>Saft</t>
+  </si>
+  <si>
+    <t>Tomate</t>
+  </si>
+  <si>
+    <t>Tanz</t>
+  </si>
+  <si>
+    <t>Hemd</t>
+  </si>
+  <si>
+    <t>Rock</t>
+  </si>
+  <si>
+    <t>Telefon</t>
+  </si>
+  <si>
+    <t>Radio</t>
+  </si>
+  <si>
+    <t>Sendung</t>
+  </si>
+  <si>
+    <t>Tanne</t>
+  </si>
+  <si>
+    <t>Hütte</t>
   </si>
 </sst>
 </file>
@@ -581,7 +581,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1001,7 +1011,7 @@
   <dimension ref="A1:D81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D81"/>
+      <selection activeCell="A2" sqref="A2:B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
@@ -1026,30 +1036,30 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -1069,47 +1079,47 @@
         <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>76</v>
+        <v>150</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -1119,147 +1129,147 @@
         <v>20</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>21</v>
+        <v>151</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="3" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -1276,140 +1286,140 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="3" t="s">
-        <v>121</v>
+        <v>152</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>122</v>
+        <v>153</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="3" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>100</v>
+        <v>154</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="3" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="3" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="3" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -1426,100 +1436,100 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2" t="s">
-        <v>36</v>
+        <v>155</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>37</v>
+        <v>156</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="4"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="3" t="s">
-        <v>125</v>
+        <v>157</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="3" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2" t="s">
-        <v>44</v>
+        <v>158</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>45</v>
+        <v>159</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -1536,60 +1546,60 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="3" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
@@ -1599,27 +1609,27 @@
         <v>14</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
@@ -1636,40 +1646,40 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="3" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="3" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="3" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
@@ -1679,7 +1689,7 @@
         <v>2</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
@@ -1689,7 +1699,7 @@
         <v>15</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
@@ -1706,136 +1716,149 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B71" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="3" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="3" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="3" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="3" t="s">
-        <v>115</v>
+        <v>160</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>116</v>
+        <v>161</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="C79" s="2"/>
       <c r="D79" s="2"/>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="3" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" s="2"/>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="3" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:D10 A12:D81 A11:C11">
-    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
+  <conditionalFormatting sqref="C2:D10 C12:D81 C11">
+    <cfRule type="duplicateValues" dxfId="12" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="15"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:D81">
+    <cfRule type="duplicateValues" dxfId="10" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="duplicateValues" dxfId="9" priority="11"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C7 C9:C81">
+    <cfRule type="duplicateValues" dxfId="8" priority="12"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D10 D12:D81">
+    <cfRule type="duplicateValues" dxfId="7" priority="13"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:B81">
+    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A81">
-    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
     <cfRule type="duplicateValues" dxfId="5" priority="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B7 B9:B81 B8:C8">
     <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:D81">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+  <conditionalFormatting sqref="B2:B81">
+    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:D10 A12:D81 A11:C11">
-    <cfRule type="duplicateValues" dxfId="2" priority="7"/>
+  <conditionalFormatting sqref="A2:B81">
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C7 C9:C81">
-    <cfRule type="duplicateValues" dxfId="1" priority="5"/>
+  <conditionalFormatting sqref="A2:B81">
+    <cfRule type="duplicateValues" dxfId="1" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D10 D12:D81">
-    <cfRule type="duplicateValues" dxfId="0" priority="6"/>
+  <conditionalFormatting sqref="A2:B81">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
laura pilot. bug fix and behavioral data
</commit_message>
<xml_diff>
--- a/cue_target_pairs.xlsx
+++ b/cue_target_pairs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\pretest_fmri\Guess_fMRI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4F72FA-7C70-49ED-97BD-B0851E5E3645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{499746FF-68E7-4ABE-90CA-A637255B0D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -426,9 +426,6 @@
     <t>Ostern</t>
   </si>
   <si>
-    <t>Schnecke</t>
-  </si>
-  <si>
     <t>Club</t>
   </si>
   <si>
@@ -483,9 +480,6 @@
     <t>Saft</t>
   </si>
   <si>
-    <t>Tomate</t>
-  </si>
-  <si>
     <t>Tanz</t>
   </si>
   <si>
@@ -511,6 +505,12 @@
   </si>
   <si>
     <t>Ferien</t>
+  </si>
+  <si>
+    <t>Wurm</t>
+  </si>
+  <si>
+    <t>Karton</t>
   </si>
 </sst>
 </file>
@@ -1060,9 +1060,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <sheetData>
@@ -1129,7 +1127,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -1179,7 +1177,7 @@
         <v>20</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -1189,7 +1187,7 @@
         <v>23</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -1199,7 +1197,7 @@
         <v>132</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -1219,7 +1217,7 @@
         <v>28</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -1246,7 +1244,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2" t="s">
-        <v>133</v>
+        <v>160</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>81</v>
@@ -1319,7 +1317,7 @@
         <v>52</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -1356,10 +1354,10 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -1379,17 +1377,17 @@
         <v>53</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -1486,10 +1484,10 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="4"/>
@@ -1499,7 +1497,7 @@
         <v>54</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -1516,7 +1514,7 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>113</v>
@@ -1539,17 +1537,17 @@
         <v>39</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -1569,7 +1567,7 @@
         <v>59</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
@@ -1599,7 +1597,7 @@
         <v>29</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
@@ -1659,7 +1657,7 @@
         <v>14</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -1739,7 +1737,7 @@
         <v>2</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
@@ -1749,7 +1747,7 @@
         <v>15</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
@@ -1806,10 +1804,10 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B75" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>147</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
@@ -1836,10 +1834,10 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
@@ -1869,27 +1867,27 @@
         <v>110</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C7 C9:C81">
-    <cfRule type="duplicateValues" dxfId="12" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="duplicateValues" dxfId="11" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:D10 C12:D81 C11">
-    <cfRule type="duplicateValues" dxfId="10" priority="21"/>
-    <cfRule type="duplicateValues" dxfId="9" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:D81">
-    <cfRule type="duplicateValues" dxfId="8" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D10 D12:D81">
-    <cfRule type="duplicateValues" dxfId="7" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:B81">
     <cfRule type="duplicateValues" dxfId="6" priority="7"/>

</xml_diff>